<commit_message>
Projekt Onlineshop FIAEB: Gantt
</commit_message>
<xml_diff>
--- a/Netzplan_Übung2.xlsx
+++ b/Netzplan_Übung2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="37">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -138,8 +138,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -334,7 +335,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,15 +347,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,16 +521,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>115200</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>264960</xdr:colOff>
-      <xdr:row>50</xdr:row>
-      <xdr:rowOff>74880</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>270720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -538,7 +539,474 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1197000" y="8202600"/>
+          <a:off x="811440" y="2264760"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2164320" y="2274480"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3516840" y="2274480"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2164320" y="3265560"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3516840" y="3265560"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>259200</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1070640" y="3265560"/>
+          <a:ext cx="282240" cy="1800"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>151560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12240</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>145440</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1082520" y="2264760"/>
+          <a:ext cx="11520" cy="984960"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4870080" y="2274480"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>1080</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6222600" y="2274480"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1080</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4869720" y="3256560"/>
+          <a:ext cx="1622880" cy="11160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>161280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>11520</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6492240" y="2274480"/>
+          <a:ext cx="11520" cy="984960"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>116280</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>266040</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>75600</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1198080" y="8212320"/>
           <a:ext cx="1773000" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -561,6 +1029,300 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="811800" y="1627920"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2164320" y="1627920"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>2520</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3516840" y="1627920"/>
+          <a:ext cx="541080" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>264600</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>271080</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>2160</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1076040" y="2602800"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>6840</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>1800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2164320" y="2602440"/>
+          <a:ext cx="276840" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>7200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>17640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1082520" y="1626120"/>
+          <a:ext cx="6480" cy="992160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>7200</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>16920</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name=""/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2435040" y="1625400"/>
+          <a:ext cx="6480" cy="992160"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25200">
+          <a:solidFill>
+            <a:srgbClr val="3465a4"/>
+          </a:solidFill>
+          <a:round/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -571,11 +1333,11 @@
   </sheetPr>
   <dimension ref="A1:AD45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F13" activeCellId="0" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="3.83"/>
   </cols>
@@ -1053,32 +1815,65 @@
         <v>0</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="12"/>
+      <c r="C13" s="12" t="n">
+        <f aca="false">A13+A15</f>
+        <v>6</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="11" t="n">
+        <f aca="false">C13</f>
+        <v>6</v>
+      </c>
       <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="H13" s="12" t="n">
+        <f aca="false">F13+F15</f>
+        <v>13</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="K13" s="11" t="n">
+        <f aca="false">H13</f>
+        <v>13</v>
+      </c>
       <c r="L13" s="4"/>
-      <c r="M13" s="4"/>
+      <c r="M13" s="12" t="n">
+        <f aca="false">K13+K15</f>
+        <v>18</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
+      <c r="P13" s="11" t="n">
+        <f aca="false">M13</f>
+        <v>18</v>
+      </c>
       <c r="Q13" s="4"/>
-      <c r="R13" s="4"/>
+      <c r="R13" s="12" t="n">
+        <f aca="false">P13+P15</f>
+        <v>21</v>
+      </c>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
-      <c r="U13" s="4"/>
+      <c r="U13" s="11" t="n">
+        <f aca="false">R13</f>
+        <v>21</v>
+      </c>
       <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
+      <c r="W13" s="12" t="n">
+        <f aca="false">U13+U15</f>
+        <v>24</v>
+      </c>
       <c r="X13" s="4"/>
       <c r="Y13" s="4"/>
-      <c r="Z13" s="4"/>
+      <c r="Z13" s="11" t="n">
+        <f aca="false">MAX(W13,R19)</f>
+        <v>26</v>
+      </c>
       <c r="AA13" s="4"/>
-      <c r="AB13" s="4"/>
+      <c r="AB13" s="12" t="n">
+        <f aca="false">Z13+Z15</f>
+        <v>35</v>
+      </c>
       <c r="AC13" s="4"/>
       <c r="AD13" s="4"/>
     </row>
@@ -1090,97 +1885,189 @@
       <c r="C14" s="13"/>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
+      <c r="F14" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
+      <c r="K14" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L14" s="13"/>
+      <c r="M14" s="13"/>
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
+      <c r="P14" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="13"/>
+      <c r="R14" s="13"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
+      <c r="U14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="V14" s="13"/>
+      <c r="W14" s="13"/>
       <c r="X14" s="4"/>
       <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="4"/>
+      <c r="Z14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
       <c r="AC14" s="4"/>
       <c r="AD14" s="4"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="n">
         <v>6</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="15" t="n">
+        <f aca="false">C16-C13</f>
+        <v>0</v>
+      </c>
+      <c r="C15" s="15" t="n">
+        <f aca="false">MIN(F13,F19)-C13</f>
+        <v>0</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="F15" s="14" t="n">
+        <f aca="false" t="array" ref="F15:F15">VLOOKUP(F14,$A$2:$H$10,8)</f>
+        <v>7</v>
+      </c>
+      <c r="G15" s="15" t="n">
+        <f aca="false">H16-H13</f>
+        <v>2</v>
+      </c>
+      <c r="H15" s="15" t="n">
+        <f aca="false">K13-H13</f>
+        <v>0</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="4"/>
+      <c r="K15" s="14" t="n">
+        <f aca="false" t="array" ref="K15:K15">VLOOKUP(K14,$A$2:$H$10,8)</f>
+        <v>5</v>
+      </c>
+      <c r="L15" s="15" t="n">
+        <f aca="false">M16-M13</f>
+        <v>2</v>
+      </c>
+      <c r="M15" s="15" t="n">
+        <f aca="false">P13-M13</f>
+        <v>0</v>
+      </c>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
-      <c r="P15" s="4"/>
-      <c r="Q15" s="4"/>
-      <c r="R15" s="4"/>
+      <c r="P15" s="14" t="n">
+        <f aca="false" t="array" ref="P15:P15">VLOOKUP(P14,$A$2:$H$10,8)</f>
+        <v>3</v>
+      </c>
+      <c r="Q15" s="15" t="n">
+        <f aca="false">R16-R13</f>
+        <v>2</v>
+      </c>
+      <c r="R15" s="15" t="n">
+        <f aca="false">U13-R13</f>
+        <v>0</v>
+      </c>
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
+      <c r="U15" s="14" t="n">
+        <f aca="false" t="array" ref="U15:U15">VLOOKUP(U14,$A$2:$H$10,8)</f>
+        <v>3</v>
+      </c>
+      <c r="V15" s="15" t="n">
+        <f aca="false">W16-W13</f>
+        <v>2</v>
+      </c>
+      <c r="W15" s="15" t="n">
+        <f aca="false">Z13-W13</f>
+        <v>2</v>
+      </c>
       <c r="X15" s="4"/>
       <c r="Y15" s="4"/>
-      <c r="Z15" s="4"/>
-      <c r="AA15" s="4"/>
-      <c r="AB15" s="4"/>
+      <c r="Z15" s="14" t="n">
+        <f aca="false" t="array" ref="Z15:Z15">VLOOKUP(Z14,$A$2:$H$10,8)</f>
+        <v>9</v>
+      </c>
+      <c r="AA15" s="15" t="n">
+        <f aca="false">AB16-AB13</f>
+        <v>0</v>
+      </c>
+      <c r="AB15" s="15"/>
       <c r="AC15" s="4"/>
       <c r="AD15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="16" t="n">
+        <f aca="false">C16-A15</f>
         <v>0</v>
       </c>
       <c r="B16" s="4"/>
-      <c r="C16" s="17"/>
+      <c r="C16" s="17" t="n">
+        <f aca="false">MIN(F16,F22)</f>
+        <v>6</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
+      <c r="F16" s="16" t="n">
+        <f aca="false">H16-F15</f>
+        <v>8</v>
+      </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
+      <c r="H16" s="17" t="n">
+        <f aca="false">K16</f>
+        <v>15</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
+      <c r="K16" s="16" t="n">
+        <f aca="false">M16-K15</f>
+        <v>15</v>
+      </c>
       <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
+      <c r="M16" s="17" t="n">
+        <f aca="false">P16</f>
+        <v>20</v>
+      </c>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
-      <c r="P16" s="4"/>
+      <c r="P16" s="16" t="n">
+        <f aca="false">R16-P15</f>
+        <v>20</v>
+      </c>
       <c r="Q16" s="4"/>
-      <c r="R16" s="4"/>
+      <c r="R16" s="17" t="n">
+        <f aca="false">U16</f>
+        <v>23</v>
+      </c>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
+      <c r="U16" s="16" t="n">
+        <f aca="false">W16-U15</f>
+        <v>23</v>
+      </c>
       <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
+      <c r="W16" s="17" t="n">
+        <f aca="false">Z16</f>
+        <v>26</v>
+      </c>
       <c r="X16" s="4"/>
       <c r="Y16" s="4"/>
-      <c r="Z16" s="4"/>
+      <c r="Z16" s="16" t="n">
+        <f aca="false">AB16-Z15</f>
+        <v>26</v>
+      </c>
       <c r="AA16" s="4"/>
-      <c r="AB16" s="4"/>
+      <c r="AB16" s="17" t="n">
+        <f aca="false">AB13</f>
+        <v>35</v>
+      </c>
       <c r="AC16" s="4"/>
       <c r="AD16" s="4"/>
     </row>
@@ -1198,6 +2085,117 @@
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
+      <c r="F19" s="11" t="n">
+        <f aca="false">C13</f>
+        <v>6</v>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="12" t="n">
+        <f aca="false">F19+F21</f>
+        <v>10</v>
+      </c>
+      <c r="K19" s="11" t="n">
+        <f aca="false">H19</f>
+        <v>10</v>
+      </c>
+      <c r="L19" s="4"/>
+      <c r="M19" s="12" t="n">
+        <f aca="false">K19+K21</f>
+        <v>19</v>
+      </c>
+      <c r="P19" s="11" t="n">
+        <f aca="false">M19</f>
+        <v>19</v>
+      </c>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="12" t="n">
+        <f aca="false">P19+P21</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="K20" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="P20" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+    </row>
+    <row r="21" customFormat="false" ht="13.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="14" t="n">
+        <f aca="false" t="array" ref="F21:F21">VLOOKUP(F20,$A$2:$H$10,8)</f>
+        <v>4</v>
+      </c>
+      <c r="G21" s="15" t="n">
+        <f aca="false">H22-H19</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="15" t="n">
+        <f aca="false">K19-H19</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="14" t="n">
+        <f aca="false" t="array" ref="K21:K21">VLOOKUP(K20,$A$2:$H$10,8)</f>
+        <v>9</v>
+      </c>
+      <c r="L21" s="15" t="n">
+        <f aca="false">M22-M19</f>
+        <v>0</v>
+      </c>
+      <c r="M21" s="15" t="n">
+        <f aca="false">P19-M19</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="14" t="n">
+        <f aca="false" t="array" ref="P21:P21">VLOOKUP(P20,$A$2:$H$10,8)</f>
+        <v>7</v>
+      </c>
+      <c r="Q21" s="15" t="n">
+        <f aca="false">R22-R19</f>
+        <v>0</v>
+      </c>
+      <c r="R21" s="15" t="n">
+        <f aca="false">Z13-R19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F22" s="16" t="n">
+        <f aca="false">H22-F21</f>
+        <v>6</v>
+      </c>
+      <c r="G22" s="4"/>
+      <c r="H22" s="17" t="n">
+        <f aca="false">K22</f>
+        <v>10</v>
+      </c>
+      <c r="K22" s="16" t="n">
+        <f aca="false">M22-K21</f>
+        <v>10</v>
+      </c>
+      <c r="L22" s="4"/>
+      <c r="M22" s="17" t="n">
+        <f aca="false">P22</f>
+        <v>19</v>
+      </c>
+      <c r="P22" s="16" t="n">
+        <f aca="false">R22-P21</f>
+        <v>19</v>
+      </c>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="17" t="n">
+        <f aca="false">Z16</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4"/>
@@ -1399,10 +2397,18 @@
       <c r="C45" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A14:C14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="U14:W14"/>
+    <mergeCell ref="Z14:AB14"/>
+    <mergeCell ref="F20:H20"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="P20:R20"/>
     <mergeCell ref="D33:H33"/>
     <mergeCell ref="A34:C34"/>
     <mergeCell ref="D34:H34"/>
@@ -1418,6 +2424,11 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B15 G15 G21 L15 L21 Q15 Q21 V15 AA15">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1425,6 +2436,7 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CSeite &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1433,13 +2445,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L63"/>
+  <dimension ref="A1:R63"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T10" activeCellId="0" sqref="T10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="3.83"/>
   </cols>
@@ -1561,8 +2573,36 @@
         <v>0</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="12" t="s">
-        <v>5</v>
+      <c r="C9" s="12" t="n">
+        <f aca="false">A9+A11</f>
+        <v>6</v>
+      </c>
+      <c r="F9" s="11" t="n">
+        <f aca="false">C9</f>
+        <v>6</v>
+      </c>
+      <c r="G9" s="4"/>
+      <c r="H9" s="12" t="n">
+        <f aca="false">F9+F11</f>
+        <v>13</v>
+      </c>
+      <c r="K9" s="11" t="n">
+        <f aca="false">MAX(H9,H15)</f>
+        <v>13</v>
+      </c>
+      <c r="L9" s="4"/>
+      <c r="M9" s="12" t="n">
+        <f aca="false">K9+K11</f>
+        <v>18</v>
+      </c>
+      <c r="P9" s="11" t="n">
+        <f aca="false">M9</f>
+        <v>18</v>
+      </c>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="12" t="n">
+        <f aca="false">P9+P11</f>
+        <v>27</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1571,25 +2611,148 @@
       </c>
       <c r="B10" s="13"/>
       <c r="C10" s="13"/>
+      <c r="F10" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="K10" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="L10" s="13"/>
+      <c r="M10" s="13"/>
+      <c r="P10" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q10" s="13"/>
+      <c r="R10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="n">
+        <f aca="false" t="array" ref="A11:A11">VLOOKUP(A10,$A$2:$H$10,8)</f>
         <v>6</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="15" t="n">
+        <f aca="false">C12-C9</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="15" t="n">
+        <f aca="false">MIN(F9,F15)-C9</f>
+        <v>0</v>
+      </c>
+      <c r="F11" s="14" t="n">
+        <f aca="false" t="array" ref="F11:F11">VLOOKUP(F10,$A$2:$H$10,8)</f>
+        <v>7</v>
+      </c>
+      <c r="G11" s="15" t="n">
+        <f aca="false">H12-H9</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="15" t="n">
+        <f aca="false">K9-H9</f>
+        <v>0</v>
+      </c>
+      <c r="K11" s="14" t="n">
+        <f aca="false" t="array" ref="K11:K11">VLOOKUP(K10,$A$2:$H$10,8)</f>
         <v>5</v>
       </c>
-      <c r="C11" s="15" t="s">
-        <v>5</v>
-      </c>
+      <c r="L11" s="15" t="n">
+        <f aca="false">M12-M9</f>
+        <v>0</v>
+      </c>
+      <c r="M11" s="15" t="n">
+        <f aca="false">P9-M9</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="14" t="n">
+        <f aca="false" t="array" ref="P11:P11">VLOOKUP(P10,$A$2:$H$10,8)</f>
+        <v>9</v>
+      </c>
+      <c r="Q11" s="15" t="n">
+        <f aca="false">R12-R9</f>
+        <v>0</v>
+      </c>
+      <c r="R11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="16" t="n">
+        <f aca="false">C12-A11</f>
         <v>0</v>
       </c>
       <c r="B12" s="4"/>
-      <c r="C12" s="17" t="s">
-        <v>5</v>
+      <c r="C12" s="17" t="n">
+        <f aca="false">MIN(F12,F18)</f>
+        <v>6</v>
+      </c>
+      <c r="F12" s="16" t="n">
+        <f aca="false">H12-F11</f>
+        <v>6</v>
+      </c>
+      <c r="G12" s="4"/>
+      <c r="H12" s="17" t="n">
+        <f aca="false">K12</f>
+        <v>13</v>
+      </c>
+      <c r="K12" s="16" t="n">
+        <f aca="false">M12-K11</f>
+        <v>13</v>
+      </c>
+      <c r="L12" s="4"/>
+      <c r="M12" s="17" t="n">
+        <f aca="false">P12</f>
+        <v>18</v>
+      </c>
+      <c r="P12" s="16" t="n">
+        <f aca="false">R12-P11</f>
+        <v>18</v>
+      </c>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="17" t="n">
+        <f aca="false">R9</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="11" t="n">
+        <f aca="false">C9</f>
+        <v>6</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="12" t="n">
+        <f aca="false">F15+F17</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F16" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="14" t="n">
+        <f aca="false" t="array" ref="F17:F17">VLOOKUP(F16,$A$2:$H$10,8)</f>
+        <v>4</v>
+      </c>
+      <c r="G17" s="15" t="n">
+        <f aca="false">H18-H15</f>
+        <v>3</v>
+      </c>
+      <c r="H17" s="15" t="n">
+        <f aca="false">K9-H15</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="16" t="n">
+        <f aca="false">H18-F17</f>
+        <v>9</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="17" t="n">
+        <f aca="false">K12</f>
+        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1835,10 +2998,14 @@
       <c r="L63" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="15">
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="A10:C10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="P10:R10"/>
+    <mergeCell ref="F16:H16"/>
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="F52:J52"/>
     <mergeCell ref="C56:K56"/>
@@ -1853,6 +3020,11 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B11 G11 G17 L11 Q11">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>